<commit_message>
averaged figures are made
</commit_message>
<xml_diff>
--- a/averages.xlsx
+++ b/averages.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="13">
   <si>
     <t>city</t>
   </si>
@@ -25,9 +25,6 @@
     <t>size</t>
   </si>
   <si>
-    <t>street</t>
-  </si>
-  <si>
     <t>price</t>
   </si>
   <si>
@@ -37,7 +34,7 @@
     <t>land_size</t>
   </si>
   <si>
-    <t>garage</t>
+    <t>count</t>
   </si>
   <si>
     <t>Date</t>
@@ -419,15 +416,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -450,91 +447,250 @@
       <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="2">
-        <v>43841.88394258471</v>
+        <v>43841</v>
       </c>
       <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2">
+        <v>118.882352941177</v>
+      </c>
+      <c r="E2">
+        <v>30002941.1764706</v>
+      </c>
+      <c r="F2">
+        <v>278100.389936275</v>
+      </c>
+      <c r="H2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="2">
+        <v>43841</v>
+      </c>
+      <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3">
+        <v>118.179487179487</v>
+      </c>
+      <c r="E3">
+        <v>24864102.5641026</v>
+      </c>
+      <c r="F3">
+        <v>215486.314278871</v>
+      </c>
+      <c r="H3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="2">
+        <v>43841</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="D2">
-        <v>118.8823529411765</v>
-      </c>
-      <c r="F2">
-        <v>30002941.17647059</v>
-      </c>
-      <c r="G2">
-        <v>278100.3899362749</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="2">
-        <v>43841.88394258471</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="D4">
+        <v>17.7551020408163</v>
+      </c>
+      <c r="E4">
+        <v>4165918.36734694</v>
+      </c>
+      <c r="F4">
+        <v>242099.910224355</v>
+      </c>
+      <c r="H4">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="2">
+        <v>43841</v>
+      </c>
+      <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5">
+        <v>160.991161616162</v>
+      </c>
+      <c r="E5">
+        <v>54929393.9393939</v>
+      </c>
+      <c r="F5">
+        <v>992379.652400437</v>
+      </c>
+      <c r="G5">
+        <v>470.02398989899</v>
+      </c>
+      <c r="H5">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="2">
+        <v>43843</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6">
+        <v>118.944444444444</v>
+      </c>
+      <c r="E6">
+        <v>29663888.8888889</v>
+      </c>
+      <c r="F6">
+        <v>273715.183087963</v>
+      </c>
+      <c r="G6">
+        <v>513.833333333333</v>
+      </c>
+      <c r="H6">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="2">
+        <v>43843</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7">
+        <v>117.475</v>
+      </c>
+      <c r="E7">
+        <v>24720000</v>
+      </c>
+      <c r="F7">
+        <v>215462.955705053</v>
+      </c>
+      <c r="G7">
+        <v>157.05</v>
+      </c>
+      <c r="H7">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="2">
+        <v>43843</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
         <v>12</v>
       </c>
-      <c r="D3">
-        <v>118.1794871794872</v>
-      </c>
-      <c r="F3">
-        <v>24864102.56410256</v>
-      </c>
-      <c r="G3">
-        <v>215486.314278871</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="2">
-        <v>43841.88394258471</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="D8">
+        <v>17.6969696969697</v>
+      </c>
+      <c r="E8">
+        <v>4154141.41414141</v>
+      </c>
+      <c r="F8">
+        <v>242309.862182307</v>
+      </c>
+      <c r="H8">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="2">
+        <v>43844</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4">
-        <v>17.75510204081633</v>
-      </c>
-      <c r="F4">
-        <v>4165918.367346939</v>
-      </c>
-      <c r="G4">
-        <v>242099.9102243548</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="2">
-        <v>43841.88394258471</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="D9">
+        <v>118.9444444444444</v>
+      </c>
+      <c r="E9">
+        <v>29663888.88888889</v>
+      </c>
+      <c r="F9">
+        <v>273715.1830879633</v>
+      </c>
+      <c r="G9">
+        <v>513.8333333333334</v>
+      </c>
+      <c r="H9">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="2">
+        <v>43844</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
         <v>11</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D10">
+        <v>117.475</v>
+      </c>
+      <c r="E10">
+        <v>24720000</v>
+      </c>
+      <c r="F10">
+        <v>215462.9557050533</v>
+      </c>
+      <c r="G10">
+        <v>157.05</v>
+      </c>
+      <c r="H10">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="2">
+        <v>43844</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
         <v>12</v>
       </c>
-      <c r="D5">
-        <v>160.9911616161616</v>
-      </c>
-      <c r="F5">
-        <v>54929393.93939394</v>
-      </c>
-      <c r="G5">
-        <v>992379.652400437</v>
-      </c>
-      <c r="H5">
-        <v>470.0239898989899</v>
+      <c r="D11">
+        <v>17.6969696969697</v>
+      </c>
+      <c r="E11">
+        <v>4154141.414141414</v>
+      </c>
+      <c r="F11">
+        <v>242309.862182307</v>
+      </c>
+      <c r="H11">
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
boxplots are added to the jupyter notebook
</commit_message>
<xml_diff>
--- a/averages.xlsx
+++ b/averages.xlsx
@@ -681,16 +681,16 @@
         <v>12</v>
       </c>
       <c r="D11">
-        <v>17.6969696969697</v>
+        <v>17.72164948453608</v>
       </c>
       <c r="E11">
-        <v>4154141.414141414</v>
+        <v>4147010.30927835</v>
       </c>
       <c r="F11">
-        <v>242309.862182307</v>
+        <v>241647.2934758712</v>
       </c>
       <c r="H11">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
temporally evolving boxplot added
</commit_message>
<xml_diff>
--- a/averages.xlsx
+++ b/averages.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="13">
   <si>
     <t>city</t>
   </si>
@@ -416,7 +416,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -693,6 +693,107 @@
         <v>97</v>
       </c>
     </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="2">
+        <v>43845</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12">
+        <v>119.1052631578947</v>
+      </c>
+      <c r="E12">
+        <v>32676315.78947368</v>
+      </c>
+      <c r="F12">
+        <v>296798.3356605554</v>
+      </c>
+      <c r="G12">
+        <v>486.8421052631579</v>
+      </c>
+      <c r="H12">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="2">
+        <v>43845</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13">
+        <v>117.475</v>
+      </c>
+      <c r="E13">
+        <v>24720000</v>
+      </c>
+      <c r="F13">
+        <v>215462.9557050533</v>
+      </c>
+      <c r="G13">
+        <v>157.05</v>
+      </c>
+      <c r="H13">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="2">
+        <v>43845</v>
+      </c>
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14">
+        <v>17.72164948453608</v>
+      </c>
+      <c r="E14">
+        <v>4147010.30927835</v>
+      </c>
+      <c r="F14">
+        <v>241647.2934758712</v>
+      </c>
+      <c r="H14">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="2">
+        <v>43845</v>
+      </c>
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15">
+        <v>161.6278195488722</v>
+      </c>
+      <c r="E15">
+        <v>55337731.82957394</v>
+      </c>
+      <c r="F15">
+        <v>989200.6957014774</v>
+      </c>
+      <c r="G15">
+        <v>466.5664160401003</v>
+      </c>
+      <c r="H15">
+        <v>798</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>